<commit_message>
Updated housing data all the way to December 2022 and reran analysis
</commit_message>
<xml_diff>
--- a/Chapter 27 - Recession Indicators/HousingNew.xlsx
+++ b/Chapter 27 - Recession Indicators/HousingNew.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walter/Desktop/SCRATCH_CODE/analytics-stories/Chapter 27 - Recession Indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9808E072-369B-F441-A6CE-2FE0CACAAF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAAF0DD-B069-C447-9D37-699CF5CB5FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61040" yWindow="500" windowWidth="32780" windowHeight="25720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22180" yWindow="500" windowWidth="28800" windowHeight="25720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
     <sheet name="up-to-date" sheetId="2" r:id="rId2"/>
+    <sheet name="latest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>FRED Graph Observations</t>
   </si>
@@ -153,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -166,6 +167,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20303,12 +20305,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6E2F6B-7CCF-E546-ABE2-62F48452FE7E}">
   <dimension ref="A1:C422"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A422" sqref="A422"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
@@ -24950,6 +24951,4788 @@
       </c>
       <c r="C422">
         <v>357.73700000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E33563E-46E4-3545-A653-1ACA7DA3CCB1}">
+  <dimension ref="A1:C433"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
+      <selection activeCell="A434" sqref="A434:XFD434"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="10">
+        <v>31778</v>
+      </c>
+      <c r="B2">
+        <v>63.733999999999902</v>
+      </c>
+      <c r="C2">
+        <v>121.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="10">
+        <v>31809</v>
+      </c>
+      <c r="B3">
+        <v>64.134</v>
+      </c>
+      <c r="C3">
+        <v>121.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="10">
+        <v>31837</v>
+      </c>
+      <c r="B4">
+        <v>64.468999999999994</v>
+      </c>
+      <c r="C4">
+        <v>121.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="10">
+        <v>31868</v>
+      </c>
+      <c r="B5">
+        <v>64.972999999999999</v>
+      </c>
+      <c r="C5">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>31898</v>
+      </c>
+      <c r="B6">
+        <v>65.546999999999997</v>
+      </c>
+      <c r="C6">
+        <v>122.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>31929</v>
+      </c>
+      <c r="B7">
+        <v>66.218000000000004</v>
+      </c>
+      <c r="C7">
+        <v>122.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="10">
+        <v>31959</v>
+      </c>
+      <c r="B8">
+        <v>66.786000000000001</v>
+      </c>
+      <c r="C8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="10">
+        <v>31990</v>
+      </c>
+      <c r="B9">
+        <v>67.268999999999906</v>
+      </c>
+      <c r="C9">
+        <v>123.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="10">
+        <v>32021</v>
+      </c>
+      <c r="B10">
+        <v>67.623000000000005</v>
+      </c>
+      <c r="C10">
+        <v>124.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="10">
+        <v>32051</v>
+      </c>
+      <c r="B11">
+        <v>67.900999999999996</v>
+      </c>
+      <c r="C11">
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="10">
+        <v>32082</v>
+      </c>
+      <c r="B12">
+        <v>68.090999999999994</v>
+      </c>
+      <c r="C12">
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="10">
+        <v>32112</v>
+      </c>
+      <c r="B13">
+        <v>68.343000000000004</v>
+      </c>
+      <c r="C13">
+        <v>125.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="10">
+        <v>32143</v>
+      </c>
+      <c r="B14">
+        <v>68.581000000000003</v>
+      </c>
+      <c r="C14">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="10">
+        <v>32174</v>
+      </c>
+      <c r="B15">
+        <v>68.914000000000001</v>
+      </c>
+      <c r="C15">
+        <v>126.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="10">
+        <v>32203</v>
+      </c>
+      <c r="B16">
+        <v>69.322999999999993</v>
+      </c>
+      <c r="C16">
+        <v>126.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="10">
+        <v>32234</v>
+      </c>
+      <c r="B17">
+        <v>69.787999999999997</v>
+      </c>
+      <c r="C17">
+        <v>126.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="10">
+        <v>32264</v>
+      </c>
+      <c r="B18">
+        <v>70.408000000000001</v>
+      </c>
+      <c r="C18">
+        <v>126.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="10">
+        <v>32295</v>
+      </c>
+      <c r="B19">
+        <v>71.066999999999993</v>
+      </c>
+      <c r="C19">
+        <v>127.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="10">
+        <v>32325</v>
+      </c>
+      <c r="B20">
+        <v>71.686000000000007</v>
+      </c>
+      <c r="C20">
+        <v>127.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="10">
+        <v>32356</v>
+      </c>
+      <c r="B21">
+        <v>72.185000000000002</v>
+      </c>
+      <c r="C21">
+        <v>128.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="10">
+        <v>32387</v>
+      </c>
+      <c r="B22">
+        <v>72.573999999999998</v>
+      </c>
+      <c r="C22">
+        <v>129.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="10">
+        <v>32417</v>
+      </c>
+      <c r="B23">
+        <v>72.822000000000003</v>
+      </c>
+      <c r="C23">
+        <v>129.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="10">
+        <v>32448</v>
+      </c>
+      <c r="B24">
+        <v>73.063999999999993</v>
+      </c>
+      <c r="C24">
+        <v>129.80000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>32478</v>
+      </c>
+      <c r="B25">
+        <v>73.277000000000001</v>
+      </c>
+      <c r="C25">
+        <v>130.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="10">
+        <v>32509</v>
+      </c>
+      <c r="B26">
+        <v>73.616</v>
+      </c>
+      <c r="C26">
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="10">
+        <v>32540</v>
+      </c>
+      <c r="B27">
+        <v>73.966999999999999</v>
+      </c>
+      <c r="C27">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="10">
+        <v>32568</v>
+      </c>
+      <c r="B28">
+        <v>74.408999999999907</v>
+      </c>
+      <c r="C28">
+        <v>131.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="10">
+        <v>32599</v>
+      </c>
+      <c r="B29">
+        <v>74.867000000000004</v>
+      </c>
+      <c r="C29">
+        <v>131.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="10">
+        <v>32629</v>
+      </c>
+      <c r="B30">
+        <v>75.295000000000002</v>
+      </c>
+      <c r="C30">
+        <v>131.69999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="10">
+        <v>32660</v>
+      </c>
+      <c r="B31">
+        <v>75.695999999999998</v>
+      </c>
+      <c r="C31">
+        <v>132.30000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="10">
+        <v>32690</v>
+      </c>
+      <c r="B32">
+        <v>76.040999999999997</v>
+      </c>
+      <c r="C32">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="10">
+        <v>32721</v>
+      </c>
+      <c r="B33">
+        <v>76.271999999999906</v>
+      </c>
+      <c r="C33">
+        <v>133.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="10">
+        <v>32752</v>
+      </c>
+      <c r="B34">
+        <v>76.421000000000006</v>
+      </c>
+      <c r="C34">
+        <v>133.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="10">
+        <v>32782</v>
+      </c>
+      <c r="B35">
+        <v>76.488</v>
+      </c>
+      <c r="C35">
+        <v>134.69999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="10">
+        <v>32813</v>
+      </c>
+      <c r="B36">
+        <v>76.521000000000001</v>
+      </c>
+      <c r="C36">
+        <v>135.19999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="10">
+        <v>32843</v>
+      </c>
+      <c r="B37">
+        <v>76.498000000000005</v>
+      </c>
+      <c r="C37">
+        <v>135.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="10">
+        <v>32874</v>
+      </c>
+      <c r="B38">
+        <v>76.527000000000001</v>
+      </c>
+      <c r="C38">
+        <v>135.80000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="10">
+        <v>32905</v>
+      </c>
+      <c r="B39">
+        <v>76.587000000000003</v>
+      </c>
+      <c r="C39">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" s="10">
+        <v>32933</v>
+      </c>
+      <c r="B40">
+        <v>76.790000000000006</v>
+      </c>
+      <c r="C40">
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="10">
+        <v>32964</v>
+      </c>
+      <c r="B41">
+        <v>77.037999999999997</v>
+      </c>
+      <c r="C41">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" s="10">
+        <v>32994</v>
+      </c>
+      <c r="B42">
+        <v>77.296000000000006</v>
+      </c>
+      <c r="C42">
+        <v>137.30000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" s="10">
+        <v>33025</v>
+      </c>
+      <c r="B43">
+        <v>77.504999999999995</v>
+      </c>
+      <c r="C43">
+        <v>137.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" s="10">
+        <v>33055</v>
+      </c>
+      <c r="B44">
+        <v>77.56</v>
+      </c>
+      <c r="C44">
+        <v>138.69999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" s="10">
+        <v>33086</v>
+      </c>
+      <c r="B45">
+        <v>77.478999999999999</v>
+      </c>
+      <c r="C45">
+        <v>139.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" s="10">
+        <v>33117</v>
+      </c>
+      <c r="B46">
+        <v>77.228999999999999</v>
+      </c>
+      <c r="C46">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" s="10">
+        <v>33147</v>
+      </c>
+      <c r="B47">
+        <v>76.911999999999907</v>
+      </c>
+      <c r="C47">
+        <v>140.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="10">
+        <v>33178</v>
+      </c>
+      <c r="B48">
+        <v>76.381</v>
+      </c>
+      <c r="C48">
+        <v>140.69999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="10">
+        <v>33208</v>
+      </c>
+      <c r="B49">
+        <v>75.971999999999994</v>
+      </c>
+      <c r="C49">
+        <v>141.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="10">
+        <v>33239</v>
+      </c>
+      <c r="B50">
+        <v>75.533000000000001</v>
+      </c>
+      <c r="C50">
+        <v>141.19999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="10">
+        <v>33270</v>
+      </c>
+      <c r="B51">
+        <v>75.248000000000005</v>
+      </c>
+      <c r="C51">
+        <v>141.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="10">
+        <v>33298</v>
+      </c>
+      <c r="B52">
+        <v>75.135999999999996</v>
+      </c>
+      <c r="C52">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53" s="10">
+        <v>33329</v>
+      </c>
+      <c r="B53">
+        <v>75.314999999999998</v>
+      </c>
+      <c r="C53">
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54" s="10">
+        <v>33359</v>
+      </c>
+      <c r="B54">
+        <v>75.768000000000001</v>
+      </c>
+      <c r="C54">
+        <v>142.80000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A55" s="10">
+        <v>33390</v>
+      </c>
+      <c r="B55">
+        <v>76.253</v>
+      </c>
+      <c r="C55">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56" s="10">
+        <v>33420</v>
+      </c>
+      <c r="B56">
+        <v>76.516999999999996</v>
+      </c>
+      <c r="C56">
+        <v>143.69999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A57" s="10">
+        <v>33451</v>
+      </c>
+      <c r="B57">
+        <v>76.593999999999994</v>
+      </c>
+      <c r="C57">
+        <v>143.69999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A58" s="10">
+        <v>33482</v>
+      </c>
+      <c r="B58">
+        <v>76.575000000000003</v>
+      </c>
+      <c r="C58">
+        <v>144.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A59" s="10">
+        <v>33512</v>
+      </c>
+      <c r="B59">
+        <v>76.290000000000006</v>
+      </c>
+      <c r="C59">
+        <v>144.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A60" s="10">
+        <v>33543</v>
+      </c>
+      <c r="B60">
+        <v>76.03</v>
+      </c>
+      <c r="C60">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A61" s="10">
+        <v>33573</v>
+      </c>
+      <c r="B61">
+        <v>75.843000000000004</v>
+      </c>
+      <c r="C61">
+        <v>145.19999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A62" s="10">
+        <v>33604</v>
+      </c>
+      <c r="B62">
+        <v>75.697999999999993</v>
+      </c>
+      <c r="C62">
+        <v>145.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A63" s="10">
+        <v>33635</v>
+      </c>
+      <c r="B63">
+        <v>75.653999999999996</v>
+      </c>
+      <c r="C63">
+        <v>145.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A64" s="10">
+        <v>33664</v>
+      </c>
+      <c r="B64">
+        <v>75.811999999999998</v>
+      </c>
+      <c r="C64">
+        <v>146.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A65" s="10">
+        <v>33695</v>
+      </c>
+      <c r="B65">
+        <v>76.078999999999994</v>
+      </c>
+      <c r="C65">
+        <v>146.19999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A66" s="10">
+        <v>33725</v>
+      </c>
+      <c r="B66">
+        <v>76.396999999999906</v>
+      </c>
+      <c r="C66">
+        <v>146.30000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A67" s="10">
+        <v>33756</v>
+      </c>
+      <c r="B67">
+        <v>76.600999999999999</v>
+      </c>
+      <c r="C67">
+        <v>146.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A68" s="10">
+        <v>33786</v>
+      </c>
+      <c r="B68">
+        <v>76.709999999999994</v>
+      </c>
+      <c r="C68">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A69" s="10">
+        <v>33817</v>
+      </c>
+      <c r="B69">
+        <v>76.730999999999995</v>
+      </c>
+      <c r="C69">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A70" s="10">
+        <v>33848</v>
+      </c>
+      <c r="B70">
+        <v>76.626999999999995</v>
+      </c>
+      <c r="C70">
+        <v>147.19999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A71" s="10">
+        <v>33878</v>
+      </c>
+      <c r="B71">
+        <v>76.596999999999994</v>
+      </c>
+      <c r="C71">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A72" s="10">
+        <v>33909</v>
+      </c>
+      <c r="B72">
+        <v>76.578000000000003</v>
+      </c>
+      <c r="C72">
+        <v>148.6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A73" s="10">
+        <v>33939</v>
+      </c>
+      <c r="B73">
+        <v>76.462999999999994</v>
+      </c>
+      <c r="C73">
+        <v>148.6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A74" s="10">
+        <v>33970</v>
+      </c>
+      <c r="B74">
+        <v>76.393999999999906</v>
+      </c>
+      <c r="C74">
+        <v>148.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A75" s="10">
+        <v>34001</v>
+      </c>
+      <c r="B75">
+        <v>76.325999999999993</v>
+      </c>
+      <c r="C75">
+        <v>149.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A76" s="10">
+        <v>34029</v>
+      </c>
+      <c r="B76">
+        <v>76.382000000000005</v>
+      </c>
+      <c r="C76">
+        <v>149.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A77" s="10">
+        <v>34060</v>
+      </c>
+      <c r="B77">
+        <v>76.66</v>
+      </c>
+      <c r="C77">
+        <v>149.69999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A78" s="10">
+        <v>34090</v>
+      </c>
+      <c r="B78">
+        <v>77.028999999999996</v>
+      </c>
+      <c r="C78">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A79" s="10">
+        <v>34121</v>
+      </c>
+      <c r="B79">
+        <v>77.515000000000001</v>
+      </c>
+      <c r="C79">
+        <v>150.30000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A80" s="10">
+        <v>34151</v>
+      </c>
+      <c r="B80">
+        <v>77.884</v>
+      </c>
+      <c r="C80">
+        <v>150.4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A81" s="10">
+        <v>34182</v>
+      </c>
+      <c r="B81">
+        <v>78.13</v>
+      </c>
+      <c r="C81">
+        <v>150.80000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A82" s="10">
+        <v>34213</v>
+      </c>
+      <c r="B82">
+        <v>78.197000000000003</v>
+      </c>
+      <c r="C82">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A83" s="10">
+        <v>34243</v>
+      </c>
+      <c r="B83">
+        <v>78.171000000000006</v>
+      </c>
+      <c r="C83">
+        <v>151.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A84" s="10">
+        <v>34274</v>
+      </c>
+      <c r="B84">
+        <v>78.168999999999997</v>
+      </c>
+      <c r="C84">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A85" s="10">
+        <v>34304</v>
+      </c>
+      <c r="B85">
+        <v>78.111999999999995</v>
+      </c>
+      <c r="C85">
+        <v>151.9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A86" s="10">
+        <v>34335</v>
+      </c>
+      <c r="B86">
+        <v>78.197999999999993</v>
+      </c>
+      <c r="C86">
+        <v>152.19999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A87" s="10">
+        <v>34366</v>
+      </c>
+      <c r="B87">
+        <v>78.203999999999994</v>
+      </c>
+      <c r="C87">
+        <v>152.80000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A88" s="10">
+        <v>34394</v>
+      </c>
+      <c r="B88">
+        <v>78.347999999999999</v>
+      </c>
+      <c r="C88">
+        <v>153.19999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A89" s="10">
+        <v>34425</v>
+      </c>
+      <c r="B89">
+        <v>78.7</v>
+      </c>
+      <c r="C89">
+        <v>153.30000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A90" s="10">
+        <v>34455</v>
+      </c>
+      <c r="B90">
+        <v>79.207999999999998</v>
+      </c>
+      <c r="C90">
+        <v>153.30000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A91" s="10">
+        <v>34486</v>
+      </c>
+      <c r="B91">
+        <v>79.7</v>
+      </c>
+      <c r="C91">
+        <v>153.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A92" s="10">
+        <v>34516</v>
+      </c>
+      <c r="B92">
+        <v>80.061999999999998</v>
+      </c>
+      <c r="C92">
+        <v>153.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A93" s="10">
+        <v>34547</v>
+      </c>
+      <c r="B93">
+        <v>80.316000000000003</v>
+      </c>
+      <c r="C93">
+        <v>154.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A94" s="10">
+        <v>34578</v>
+      </c>
+      <c r="B94">
+        <v>80.338999999999999</v>
+      </c>
+      <c r="C94">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A95" s="10">
+        <v>34608</v>
+      </c>
+      <c r="B95">
+        <v>80.302999999999997</v>
+      </c>
+      <c r="C95">
+        <v>155.19999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A96" s="10">
+        <v>34639</v>
+      </c>
+      <c r="B96">
+        <v>80.168000000000006</v>
+      </c>
+      <c r="C96">
+        <v>155.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A97" s="10">
+        <v>34669</v>
+      </c>
+      <c r="B97">
+        <v>80.076999999999998</v>
+      </c>
+      <c r="C97">
+        <v>155.69999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A98" s="10">
+        <v>34700</v>
+      </c>
+      <c r="B98">
+        <v>80.025999999999996</v>
+      </c>
+      <c r="C98">
+        <v>156.1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A99" s="10">
+        <v>34731</v>
+      </c>
+      <c r="B99">
+        <v>79.991</v>
+      </c>
+      <c r="C99">
+        <v>156.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A100" s="10">
+        <v>34759</v>
+      </c>
+      <c r="B100">
+        <v>80.076999999999998</v>
+      </c>
+      <c r="C100">
+        <v>156.69999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A101" s="10">
+        <v>34790</v>
+      </c>
+      <c r="B101">
+        <v>80.369</v>
+      </c>
+      <c r="C101">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A102" s="10">
+        <v>34820</v>
+      </c>
+      <c r="B102">
+        <v>80.691000000000003</v>
+      </c>
+      <c r="C102">
+        <v>157.19999999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A103" s="10">
+        <v>34851</v>
+      </c>
+      <c r="B103">
+        <v>81.067999999999998</v>
+      </c>
+      <c r="C103">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A104" s="10">
+        <v>34881</v>
+      </c>
+      <c r="B104">
+        <v>81.411999999999907</v>
+      </c>
+      <c r="C104">
+        <v>157.9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A105" s="10">
+        <v>34912</v>
+      </c>
+      <c r="B105">
+        <v>81.653999999999996</v>
+      </c>
+      <c r="C105">
+        <v>158.19999999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A106" s="10">
+        <v>34943</v>
+      </c>
+      <c r="B106">
+        <v>81.738</v>
+      </c>
+      <c r="C106">
+        <v>158.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A107" s="10">
+        <v>34973</v>
+      </c>
+      <c r="B107">
+        <v>81.727000000000004</v>
+      </c>
+      <c r="C107">
+        <v>158.9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A108" s="10">
+        <v>35004</v>
+      </c>
+      <c r="B108">
+        <v>81.631</v>
+      </c>
+      <c r="C108">
+        <v>159.30000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A109" s="10">
+        <v>35034</v>
+      </c>
+      <c r="B109">
+        <v>81.513000000000005</v>
+      </c>
+      <c r="C109">
+        <v>159.6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A110" s="10">
+        <v>35065</v>
+      </c>
+      <c r="B110">
+        <v>81.426999999999893</v>
+      </c>
+      <c r="C110">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A111" s="10">
+        <v>35096</v>
+      </c>
+      <c r="B111">
+        <v>81.399000000000001</v>
+      </c>
+      <c r="C111">
+        <v>160.4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A112" s="10">
+        <v>35125</v>
+      </c>
+      <c r="B112">
+        <v>81.665000000000006</v>
+      </c>
+      <c r="C112">
+        <v>160.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A113" s="10">
+        <v>35156</v>
+      </c>
+      <c r="B113">
+        <v>82.123999999999995</v>
+      </c>
+      <c r="C113">
+        <v>160.9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A114" s="10">
+        <v>35186</v>
+      </c>
+      <c r="B114">
+        <v>82.600999999999999</v>
+      </c>
+      <c r="C114">
+        <v>161.19999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A115" s="10">
+        <v>35217</v>
+      </c>
+      <c r="B115">
+        <v>83.047999999999902</v>
+      </c>
+      <c r="C115">
+        <v>161.69999999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A116" s="10">
+        <v>35247</v>
+      </c>
+      <c r="B116">
+        <v>83.417999999999907</v>
+      </c>
+      <c r="C116">
+        <v>162.19999999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A117" s="10">
+        <v>35278</v>
+      </c>
+      <c r="B117">
+        <v>83.643999999999906</v>
+      </c>
+      <c r="C117">
+        <v>162.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A118" s="10">
+        <v>35309</v>
+      </c>
+      <c r="B118">
+        <v>83.700999999999993</v>
+      </c>
+      <c r="C118">
+        <v>162.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A119" s="10">
+        <v>35339</v>
+      </c>
+      <c r="B119">
+        <v>83.627999999999901</v>
+      </c>
+      <c r="C119">
+        <v>163.30000000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A120" s="10">
+        <v>35370</v>
+      </c>
+      <c r="B120">
+        <v>83.555000000000007</v>
+      </c>
+      <c r="C120">
+        <v>163.69999999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A121" s="10">
+        <v>35400</v>
+      </c>
+      <c r="B121">
+        <v>83.49</v>
+      </c>
+      <c r="C121">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A122" s="10">
+        <v>35431</v>
+      </c>
+      <c r="B122">
+        <v>83.53</v>
+      </c>
+      <c r="C122">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A123" s="10">
+        <v>35462</v>
+      </c>
+      <c r="B123">
+        <v>83.596000000000004</v>
+      </c>
+      <c r="C123">
+        <v>164.8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A124" s="10">
+        <v>35490</v>
+      </c>
+      <c r="B124">
+        <v>83.911000000000001</v>
+      </c>
+      <c r="C124">
+        <v>165.1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A125" s="10">
+        <v>35521</v>
+      </c>
+      <c r="B125">
+        <v>84.32</v>
+      </c>
+      <c r="C125">
+        <v>165.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A126" s="10">
+        <v>35551</v>
+      </c>
+      <c r="B126">
+        <v>84.863</v>
+      </c>
+      <c r="C126">
+        <v>165.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A127" s="10">
+        <v>35582</v>
+      </c>
+      <c r="B127">
+        <v>85.397000000000006</v>
+      </c>
+      <c r="C127">
+        <v>166.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A128" s="10">
+        <v>35612</v>
+      </c>
+      <c r="B128">
+        <v>85.84</v>
+      </c>
+      <c r="C128">
+        <v>166.8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A129" s="10">
+        <v>35643</v>
+      </c>
+      <c r="B129">
+        <v>86.15</v>
+      </c>
+      <c r="C129">
+        <v>167.3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A130" s="10">
+        <v>35674</v>
+      </c>
+      <c r="B130">
+        <v>86.31</v>
+      </c>
+      <c r="C130">
+        <v>167.8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A131" s="10">
+        <v>35704</v>
+      </c>
+      <c r="B131">
+        <v>86.406999999999996</v>
+      </c>
+      <c r="C131">
+        <v>168.2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A132" s="10">
+        <v>35735</v>
+      </c>
+      <c r="B132">
+        <v>86.631</v>
+      </c>
+      <c r="C132">
+        <v>168.7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A133" s="10">
+        <v>35765</v>
+      </c>
+      <c r="B133">
+        <v>86.846999999999994</v>
+      </c>
+      <c r="C133">
+        <v>169.1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A134" s="10">
+        <v>35796</v>
+      </c>
+      <c r="B134">
+        <v>87.162000000000006</v>
+      </c>
+      <c r="C134">
+        <v>169.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A135" s="10">
+        <v>35827</v>
+      </c>
+      <c r="B135">
+        <v>87.372</v>
+      </c>
+      <c r="C135">
+        <v>169.9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A136" s="10">
+        <v>35855</v>
+      </c>
+      <c r="B136">
+        <v>87.876000000000005</v>
+      </c>
+      <c r="C136">
+        <v>170.3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A137" s="10">
+        <v>35886</v>
+      </c>
+      <c r="B137">
+        <v>88.557000000000002</v>
+      </c>
+      <c r="C137">
+        <v>170.7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A138" s="10">
+        <v>35916</v>
+      </c>
+      <c r="B138">
+        <v>89.372999999999905</v>
+      </c>
+      <c r="C138">
+        <v>171.1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A139" s="10">
+        <v>35947</v>
+      </c>
+      <c r="B139">
+        <v>90.194000000000003</v>
+      </c>
+      <c r="C139">
+        <v>171.7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A140" s="10">
+        <v>35977</v>
+      </c>
+      <c r="B140">
+        <v>90.857999999999905</v>
+      </c>
+      <c r="C140">
+        <v>172.2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A141" s="10">
+        <v>36008</v>
+      </c>
+      <c r="B141">
+        <v>91.406000000000006</v>
+      </c>
+      <c r="C141">
+        <v>172.8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A142" s="10">
+        <v>36039</v>
+      </c>
+      <c r="B142">
+        <v>91.751000000000005</v>
+      </c>
+      <c r="C142">
+        <v>173.4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A143" s="10">
+        <v>36069</v>
+      </c>
+      <c r="B143">
+        <v>91.998999999999995</v>
+      </c>
+      <c r="C143">
+        <v>173.9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A144" s="10">
+        <v>36100</v>
+      </c>
+      <c r="B144">
+        <v>92.195999999999998</v>
+      </c>
+      <c r="C144">
+        <v>174.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A145" s="10">
+        <v>36130</v>
+      </c>
+      <c r="B145">
+        <v>92.442999999999998</v>
+      </c>
+      <c r="C145">
+        <v>174.9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A146" s="10">
+        <v>36161</v>
+      </c>
+      <c r="B146">
+        <v>92.712999999999994</v>
+      </c>
+      <c r="C146">
+        <v>175.3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A147" s="10">
+        <v>36192</v>
+      </c>
+      <c r="B147">
+        <v>92.978999999999999</v>
+      </c>
+      <c r="C147">
+        <v>175.6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A148" s="10">
+        <v>36220</v>
+      </c>
+      <c r="B148">
+        <v>93.61</v>
+      </c>
+      <c r="C148">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A149" s="10">
+        <v>36251</v>
+      </c>
+      <c r="B149">
+        <v>94.435000000000002</v>
+      </c>
+      <c r="C149">
+        <v>176.4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A150" s="10">
+        <v>36281</v>
+      </c>
+      <c r="B150">
+        <v>95.358999999999995</v>
+      </c>
+      <c r="C150">
+        <v>176.7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A151" s="10">
+        <v>36312</v>
+      </c>
+      <c r="B151">
+        <v>96.361999999999995</v>
+      </c>
+      <c r="C151">
+        <v>177.1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A152" s="10">
+        <v>36342</v>
+      </c>
+      <c r="B152">
+        <v>97.191000000000003</v>
+      </c>
+      <c r="C152">
+        <v>177.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A153" s="10">
+        <v>36373</v>
+      </c>
+      <c r="B153">
+        <v>97.896000000000001</v>
+      </c>
+      <c r="C153">
+        <v>177.9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A154" s="10">
+        <v>36404</v>
+      </c>
+      <c r="B154">
+        <v>98.399000000000001</v>
+      </c>
+      <c r="C154">
+        <v>178.4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A155" s="10">
+        <v>36434</v>
+      </c>
+      <c r="B155">
+        <v>98.831000000000003</v>
+      </c>
+      <c r="C155">
+        <v>178.8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A156" s="10">
+        <v>36465</v>
+      </c>
+      <c r="B156">
+        <v>99.147999999999996</v>
+      </c>
+      <c r="C156">
+        <v>179.8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A157" s="10">
+        <v>36495</v>
+      </c>
+      <c r="B157">
+        <v>99.542000000000002</v>
+      </c>
+      <c r="C157">
+        <v>180.3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A158" s="10">
+        <v>36526</v>
+      </c>
+      <c r="B158">
+        <v>100</v>
+      </c>
+      <c r="C158">
+        <v>181.1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A159" s="10">
+        <v>36557</v>
+      </c>
+      <c r="B159">
+        <v>100.571</v>
+      </c>
+      <c r="C159">
+        <v>181.5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A160" s="10">
+        <v>36586</v>
+      </c>
+      <c r="B160">
+        <v>101.46599999999999</v>
+      </c>
+      <c r="C160">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A161" s="10">
+        <v>36617</v>
+      </c>
+      <c r="B161">
+        <v>102.541</v>
+      </c>
+      <c r="C161">
+        <v>182.3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A162" s="10">
+        <v>36647</v>
+      </c>
+      <c r="B162">
+        <v>103.702</v>
+      </c>
+      <c r="C162">
+        <v>182.7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A163" s="10">
+        <v>36678</v>
+      </c>
+      <c r="B163">
+        <v>104.855</v>
+      </c>
+      <c r="C163">
+        <v>183.2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A164" s="10">
+        <v>36708</v>
+      </c>
+      <c r="B164">
+        <v>105.72199999999999</v>
+      </c>
+      <c r="C164">
+        <v>183.9</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A165" s="10">
+        <v>36739</v>
+      </c>
+      <c r="B165">
+        <v>106.52200000000001</v>
+      </c>
+      <c r="C165">
+        <v>184.6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A166" s="10">
+        <v>36770</v>
+      </c>
+      <c r="B166">
+        <v>107.13500000000001</v>
+      </c>
+      <c r="C166">
+        <v>185.3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A167" s="10">
+        <v>36800</v>
+      </c>
+      <c r="B167">
+        <v>107.72799999999999</v>
+      </c>
+      <c r="C167">
+        <v>186.1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A168" s="10">
+        <v>36831</v>
+      </c>
+      <c r="B168">
+        <v>108.291</v>
+      </c>
+      <c r="C168">
+        <v>186.8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A169" s="10">
+        <v>36861</v>
+      </c>
+      <c r="B169">
+        <v>108.791</v>
+      </c>
+      <c r="C169">
+        <v>187.6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A170" s="10">
+        <v>36892</v>
+      </c>
+      <c r="B170">
+        <v>109.214</v>
+      </c>
+      <c r="C170">
+        <v>188.2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A171" s="10">
+        <v>36923</v>
+      </c>
+      <c r="B171">
+        <v>109.642</v>
+      </c>
+      <c r="C171">
+        <v>188.9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A172" s="10">
+        <v>36951</v>
+      </c>
+      <c r="B172">
+        <v>110.393999999999</v>
+      </c>
+      <c r="C172">
+        <v>189.6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A173" s="10">
+        <v>36982</v>
+      </c>
+      <c r="B173">
+        <v>111.247</v>
+      </c>
+      <c r="C173">
+        <v>190.2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A174" s="10">
+        <v>37012</v>
+      </c>
+      <c r="B174">
+        <v>112.202</v>
+      </c>
+      <c r="C174">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A175" s="10">
+        <v>37043</v>
+      </c>
+      <c r="B175">
+        <v>113.27200000000001</v>
+      </c>
+      <c r="C175">
+        <v>191.6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A176" s="10">
+        <v>37073</v>
+      </c>
+      <c r="B176">
+        <v>114.226</v>
+      </c>
+      <c r="C176">
+        <v>192.3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A177" s="10">
+        <v>37104</v>
+      </c>
+      <c r="B177">
+        <v>114.98699999999999</v>
+      </c>
+      <c r="C177">
+        <v>193.1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A178" s="10">
+        <v>37135</v>
+      </c>
+      <c r="B178">
+        <v>115.465</v>
+      </c>
+      <c r="C178">
+        <v>193.9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A179" s="10">
+        <v>37165</v>
+      </c>
+      <c r="B179">
+        <v>115.681</v>
+      </c>
+      <c r="C179">
+        <v>194.7</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A180" s="10">
+        <v>37196</v>
+      </c>
+      <c r="B180">
+        <v>115.83799999999999</v>
+      </c>
+      <c r="C180">
+        <v>195.5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A181" s="10">
+        <v>37226</v>
+      </c>
+      <c r="B181">
+        <v>116.056</v>
+      </c>
+      <c r="C181">
+        <v>196.4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A182" s="10">
+        <v>37257</v>
+      </c>
+      <c r="B182">
+        <v>116.437</v>
+      </c>
+      <c r="C182">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A183" s="10">
+        <v>37288</v>
+      </c>
+      <c r="B183">
+        <v>116.917</v>
+      </c>
+      <c r="C183">
+        <v>197.7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A184" s="10">
+        <v>37316</v>
+      </c>
+      <c r="B184">
+        <v>117.93</v>
+      </c>
+      <c r="C184">
+        <v>198.2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A185" s="10">
+        <v>37347</v>
+      </c>
+      <c r="B185">
+        <v>119.209</v>
+      </c>
+      <c r="C185">
+        <v>198.5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A186" s="10">
+        <v>37377</v>
+      </c>
+      <c r="B186">
+        <v>120.788</v>
+      </c>
+      <c r="C186">
+        <v>198.8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A187" s="10">
+        <v>37408</v>
+      </c>
+      <c r="B187">
+        <v>122.333</v>
+      </c>
+      <c r="C187">
+        <v>199.3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A188" s="10">
+        <v>37438</v>
+      </c>
+      <c r="B188">
+        <v>123.687</v>
+      </c>
+      <c r="C188">
+        <v>199.8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A189" s="10">
+        <v>37469</v>
+      </c>
+      <c r="B189">
+        <v>124.73</v>
+      </c>
+      <c r="C189">
+        <v>200.2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A190" s="10">
+        <v>37500</v>
+      </c>
+      <c r="B190">
+        <v>125.494</v>
+      </c>
+      <c r="C190">
+        <v>200.7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A191" s="10">
+        <v>37530</v>
+      </c>
+      <c r="B191">
+        <v>126.136</v>
+      </c>
+      <c r="C191">
+        <v>201.3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A192" s="10">
+        <v>37561</v>
+      </c>
+      <c r="B192">
+        <v>126.642</v>
+      </c>
+      <c r="C192">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A193" s="10">
+        <v>37591</v>
+      </c>
+      <c r="B193">
+        <v>127.15</v>
+      </c>
+      <c r="C193">
+        <v>202.5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A194" s="10">
+        <v>37622</v>
+      </c>
+      <c r="B194">
+        <v>127.652</v>
+      </c>
+      <c r="C194">
+        <v>203.3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A195" s="10">
+        <v>37653</v>
+      </c>
+      <c r="B195">
+        <v>128.32599999999999</v>
+      </c>
+      <c r="C195">
+        <v>203.7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A196" s="10">
+        <v>37681</v>
+      </c>
+      <c r="B196">
+        <v>129.30799999999999</v>
+      </c>
+      <c r="C196">
+        <v>204.1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A197" s="10">
+        <v>37712</v>
+      </c>
+      <c r="B197">
+        <v>130.488</v>
+      </c>
+      <c r="C197">
+        <v>204.5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A198" s="10">
+        <v>37742</v>
+      </c>
+      <c r="B198">
+        <v>131.839</v>
+      </c>
+      <c r="C198">
+        <v>204.9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A199" s="10">
+        <v>37773</v>
+      </c>
+      <c r="B199">
+        <v>133.22499999999999</v>
+      </c>
+      <c r="C199">
+        <v>205.1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A200" s="10">
+        <v>37803</v>
+      </c>
+      <c r="B200">
+        <v>134.64699999999999</v>
+      </c>
+      <c r="C200">
+        <v>205.6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A201" s="10">
+        <v>37834</v>
+      </c>
+      <c r="B201">
+        <v>135.96600000000001</v>
+      </c>
+      <c r="C201">
+        <v>206.1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A202" s="10">
+        <v>37865</v>
+      </c>
+      <c r="B202">
+        <v>137.077</v>
+      </c>
+      <c r="C202">
+        <v>206.6</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A203" s="10">
+        <v>37895</v>
+      </c>
+      <c r="B203">
+        <v>137.976</v>
+      </c>
+      <c r="C203">
+        <v>206.9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A204" s="10">
+        <v>37926</v>
+      </c>
+      <c r="B204">
+        <v>138.76499999999999</v>
+      </c>
+      <c r="C204">
+        <v>207.5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A205" s="10">
+        <v>37956</v>
+      </c>
+      <c r="B205">
+        <v>139.62799999999999</v>
+      </c>
+      <c r="C205">
+        <v>207.9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A206" s="10">
+        <v>37987</v>
+      </c>
+      <c r="B206">
+        <v>140.70599999999999</v>
+      </c>
+      <c r="C206">
+        <v>208.3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A207" s="10">
+        <v>38018</v>
+      </c>
+      <c r="B207">
+        <v>142.029</v>
+      </c>
+      <c r="C207">
+        <v>208.8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A208" s="10">
+        <v>38047</v>
+      </c>
+      <c r="B208">
+        <v>144.08000000000001</v>
+      </c>
+      <c r="C208">
+        <v>209.2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A209" s="10">
+        <v>38078</v>
+      </c>
+      <c r="B209">
+        <v>146.18</v>
+      </c>
+      <c r="C209">
+        <v>209.7</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A210" s="10">
+        <v>38108</v>
+      </c>
+      <c r="B210">
+        <v>148.334</v>
+      </c>
+      <c r="C210">
+        <v>210.2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A211" s="10">
+        <v>38139</v>
+      </c>
+      <c r="B211">
+        <v>150.518</v>
+      </c>
+      <c r="C211">
+        <v>210.7</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A212" s="10">
+        <v>38169</v>
+      </c>
+      <c r="B212">
+        <v>152.33699999999999</v>
+      </c>
+      <c r="C212">
+        <v>211.2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A213" s="10">
+        <v>38200</v>
+      </c>
+      <c r="B213">
+        <v>153.81399999999999</v>
+      </c>
+      <c r="C213">
+        <v>211.9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A214" s="10">
+        <v>38231</v>
+      </c>
+      <c r="B214">
+        <v>155.108</v>
+      </c>
+      <c r="C214">
+        <v>212.4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A215" s="10">
+        <v>38261</v>
+      </c>
+      <c r="B215">
+        <v>156.298</v>
+      </c>
+      <c r="C215">
+        <v>212.8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A216" s="10">
+        <v>38292</v>
+      </c>
+      <c r="B216">
+        <v>157.49600000000001</v>
+      </c>
+      <c r="C216">
+        <v>213.2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A217" s="10">
+        <v>38322</v>
+      </c>
+      <c r="B217">
+        <v>158.66999999999999</v>
+      </c>
+      <c r="C217">
+        <v>213.9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A218" s="10">
+        <v>38353</v>
+      </c>
+      <c r="B218">
+        <v>160.13</v>
+      </c>
+      <c r="C218">
+        <v>214.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A219" s="10">
+        <v>38384</v>
+      </c>
+      <c r="B219">
+        <v>161.92500000000001</v>
+      </c>
+      <c r="C219">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A220" s="10">
+        <v>38412</v>
+      </c>
+      <c r="B220">
+        <v>164.57599999999999</v>
+      </c>
+      <c r="C220">
+        <v>215.5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A221" s="10">
+        <v>38443</v>
+      </c>
+      <c r="B221">
+        <v>166.999</v>
+      </c>
+      <c r="C221">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A222" s="10">
+        <v>38473</v>
+      </c>
+      <c r="B222">
+        <v>169.54400000000001</v>
+      </c>
+      <c r="C222">
+        <v>216.4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A223" s="10">
+        <v>38504</v>
+      </c>
+      <c r="B223">
+        <v>172.01599999999999</v>
+      </c>
+      <c r="C223">
+        <v>216.8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A224" s="10">
+        <v>38534</v>
+      </c>
+      <c r="B224">
+        <v>174.09799999999899</v>
+      </c>
+      <c r="C224">
+        <v>217.5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A225" s="10">
+        <v>38565</v>
+      </c>
+      <c r="B225">
+        <v>175.92400000000001</v>
+      </c>
+      <c r="C225">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A226" s="10">
+        <v>38596</v>
+      </c>
+      <c r="B226">
+        <v>177.61099999999999</v>
+      </c>
+      <c r="C226">
+        <v>218.6</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A227" s="10">
+        <v>38626</v>
+      </c>
+      <c r="B227">
+        <v>178.75200000000001</v>
+      </c>
+      <c r="C227">
+        <v>219.3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A228" s="10">
+        <v>38657</v>
+      </c>
+      <c r="B228">
+        <v>179.673</v>
+      </c>
+      <c r="C228">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A229" s="10">
+        <v>38687</v>
+      </c>
+      <c r="B229">
+        <v>180.107</v>
+      </c>
+      <c r="C229">
+        <v>220.5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A230" s="10">
+        <v>38718</v>
+      </c>
+      <c r="B230">
+        <v>180.828</v>
+      </c>
+      <c r="C230">
+        <v>220.9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A231" s="10">
+        <v>38749</v>
+      </c>
+      <c r="B231">
+        <v>181.50099999999901</v>
+      </c>
+      <c r="C231">
+        <v>221.6</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A232" s="10">
+        <v>38777</v>
+      </c>
+      <c r="B232">
+        <v>182.75</v>
+      </c>
+      <c r="C232">
+        <v>222.3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A233" s="10">
+        <v>38808</v>
+      </c>
+      <c r="B233">
+        <v>183.648</v>
+      </c>
+      <c r="C233">
+        <v>222.9</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A234" s="10">
+        <v>38838</v>
+      </c>
+      <c r="B234">
+        <v>184.37899999999999</v>
+      </c>
+      <c r="C234">
+        <v>223.6</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A235" s="10">
+        <v>38869</v>
+      </c>
+      <c r="B235">
+        <v>184.547</v>
+      </c>
+      <c r="C235">
+        <v>224.4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A236" s="10">
+        <v>38899</v>
+      </c>
+      <c r="B236">
+        <v>184.607</v>
+      </c>
+      <c r="C236">
+        <v>225.2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A237" s="10">
+        <v>38930</v>
+      </c>
+      <c r="B237">
+        <v>184.404</v>
+      </c>
+      <c r="C237">
+        <v>226.2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A238" s="10">
+        <v>38961</v>
+      </c>
+      <c r="B238">
+        <v>184.19799999999901</v>
+      </c>
+      <c r="C238">
+        <v>227.1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A239" s="10">
+        <v>38991</v>
+      </c>
+      <c r="B239">
+        <v>184.054</v>
+      </c>
+      <c r="C239">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A240" s="10">
+        <v>39022</v>
+      </c>
+      <c r="B240">
+        <v>183.63200000000001</v>
+      </c>
+      <c r="C240">
+        <v>228.9</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A241" s="10">
+        <v>39052</v>
+      </c>
+      <c r="B241">
+        <v>183.23</v>
+      </c>
+      <c r="C241">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A242" s="10">
+        <v>39083</v>
+      </c>
+      <c r="B242">
+        <v>182.71899999999999</v>
+      </c>
+      <c r="C242">
+        <v>230.80600000000001</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A243" s="10">
+        <v>39114</v>
+      </c>
+      <c r="B243">
+        <v>182.47200000000001</v>
+      </c>
+      <c r="C243">
+        <v>231.739</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A244" s="10">
+        <v>39142</v>
+      </c>
+      <c r="B244">
+        <v>182.19399999999999</v>
+      </c>
+      <c r="C244">
+        <v>232.495</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A245" s="10">
+        <v>39173</v>
+      </c>
+      <c r="B245">
+        <v>182.13099999999901</v>
+      </c>
+      <c r="C245">
+        <v>232.98</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A246" s="10">
+        <v>39203</v>
+      </c>
+      <c r="B246">
+        <v>181.88399999999999</v>
+      </c>
+      <c r="C246">
+        <v>233.54900000000001</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A247" s="10">
+        <v>39234</v>
+      </c>
+      <c r="B247">
+        <v>181.54</v>
+      </c>
+      <c r="C247">
+        <v>234.071</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A248" s="10">
+        <v>39264</v>
+      </c>
+      <c r="B248">
+        <v>180.99299999999999</v>
+      </c>
+      <c r="C248">
+        <v>234.732</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A249" s="10">
+        <v>39295</v>
+      </c>
+      <c r="B249">
+        <v>180.23400000000001</v>
+      </c>
+      <c r="C249">
+        <v>235.31100000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A250" s="10">
+        <v>39326</v>
+      </c>
+      <c r="B250">
+        <v>179.12200000000001</v>
+      </c>
+      <c r="C250">
+        <v>236.05799999999999</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A251" s="10">
+        <v>39356</v>
+      </c>
+      <c r="B251">
+        <v>177.53</v>
+      </c>
+      <c r="C251">
+        <v>237.13499999999999</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A252" s="10">
+        <v>39387</v>
+      </c>
+      <c r="B252">
+        <v>175.16200000000001</v>
+      </c>
+      <c r="C252">
+        <v>238.16900000000001</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A253" s="10">
+        <v>39417</v>
+      </c>
+      <c r="B253">
+        <v>173.33799999999999</v>
+      </c>
+      <c r="C253">
+        <v>239.102</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A254" s="10">
+        <v>39448</v>
+      </c>
+      <c r="B254">
+        <v>171.078</v>
+      </c>
+      <c r="C254">
+        <v>239.85</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A255" s="10">
+        <v>39479</v>
+      </c>
+      <c r="B255">
+        <v>169.19200000000001</v>
+      </c>
+      <c r="C255">
+        <v>240.32499999999999</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A256" s="10">
+        <v>39508</v>
+      </c>
+      <c r="B256">
+        <v>167.905</v>
+      </c>
+      <c r="C256">
+        <v>240.874</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A257" s="10">
+        <v>39539</v>
+      </c>
+      <c r="B257">
+        <v>167.32499999999999</v>
+      </c>
+      <c r="C257">
+        <v>241.47399999999999</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A258" s="10">
+        <v>39569</v>
+      </c>
+      <c r="B258">
+        <v>167.02199999999999</v>
+      </c>
+      <c r="C258">
+        <v>241.803</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A259" s="10">
+        <v>39600</v>
+      </c>
+      <c r="B259">
+        <v>166.53799999999899</v>
+      </c>
+      <c r="C259">
+        <v>242.64</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A260" s="10">
+        <v>39630</v>
+      </c>
+      <c r="B260">
+        <v>165.714</v>
+      </c>
+      <c r="C260">
+        <v>243.36699999999999</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A261" s="10">
+        <v>39661</v>
+      </c>
+      <c r="B261">
+        <v>164.27799999999999</v>
+      </c>
+      <c r="C261">
+        <v>244.18100000000001</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A262" s="10">
+        <v>39692</v>
+      </c>
+      <c r="B262">
+        <v>161.91299999999899</v>
+      </c>
+      <c r="C262">
+        <v>244.92599999999999</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A263" s="10">
+        <v>39722</v>
+      </c>
+      <c r="B263">
+        <v>159.16299999999899</v>
+      </c>
+      <c r="C263">
+        <v>245.85499999999999</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A264" s="10">
+        <v>39753</v>
+      </c>
+      <c r="B264">
+        <v>156.071</v>
+      </c>
+      <c r="C264">
+        <v>246.68100000000001</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A265" s="10">
+        <v>39783</v>
+      </c>
+      <c r="B265">
+        <v>152.54399999999899</v>
+      </c>
+      <c r="C265">
+        <v>247.27799999999999</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A266" s="10">
+        <v>39814</v>
+      </c>
+      <c r="B266">
+        <v>149.36199999999999</v>
+      </c>
+      <c r="C266">
+        <v>247.97399999999999</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A267" s="10">
+        <v>39845</v>
+      </c>
+      <c r="B267">
+        <v>147.61699999999999</v>
+      </c>
+      <c r="C267">
+        <v>248.30500000000001</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A268" s="10">
+        <v>39873</v>
+      </c>
+      <c r="B268">
+        <v>146.51400000000001</v>
+      </c>
+      <c r="C268">
+        <v>248.63900000000001</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A269" s="10">
+        <v>39904</v>
+      </c>
+      <c r="B269">
+        <v>146.94299999999899</v>
+      </c>
+      <c r="C269">
+        <v>248.899</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A270" s="10">
+        <v>39934</v>
+      </c>
+      <c r="B270">
+        <v>148.16999999999999</v>
+      </c>
+      <c r="C270">
+        <v>249.06899999999999</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A271" s="10">
+        <v>39965</v>
+      </c>
+      <c r="B271">
+        <v>149.797</v>
+      </c>
+      <c r="C271">
+        <v>249.09200000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A272" s="10">
+        <v>39995</v>
+      </c>
+      <c r="B272">
+        <v>150.749</v>
+      </c>
+      <c r="C272">
+        <v>248.994</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A273" s="10">
+        <v>40026</v>
+      </c>
+      <c r="B273">
+        <v>150.66800000000001</v>
+      </c>
+      <c r="C273">
+        <v>249.029</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A274" s="10">
+        <v>40057</v>
+      </c>
+      <c r="B274">
+        <v>149.626</v>
+      </c>
+      <c r="C274">
+        <v>248.965</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A275" s="10">
+        <v>40087</v>
+      </c>
+      <c r="B275">
+        <v>148.583</v>
+      </c>
+      <c r="C275">
+        <v>248.88800000000001</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A276" s="10">
+        <v>40118</v>
+      </c>
+      <c r="B276">
+        <v>147.93799999999999</v>
+      </c>
+      <c r="C276">
+        <v>248.886</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A277" s="10">
+        <v>40148</v>
+      </c>
+      <c r="B277">
+        <v>146.66399999999999</v>
+      </c>
+      <c r="C277">
+        <v>248.999</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A278" s="10">
+        <v>40179</v>
+      </c>
+      <c r="B278">
+        <v>145.00299999999999</v>
+      </c>
+      <c r="C278">
+        <v>249.14400000000001</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A279" s="10">
+        <v>40210</v>
+      </c>
+      <c r="B279">
+        <v>143.05500000000001</v>
+      </c>
+      <c r="C279">
+        <v>249.017</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A280" s="10">
+        <v>40238</v>
+      </c>
+      <c r="B280">
+        <v>143.59700000000001</v>
+      </c>
+      <c r="C280">
+        <v>249.089</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A281" s="10">
+        <v>40269</v>
+      </c>
+      <c r="B281">
+        <v>145.40299999999999</v>
+      </c>
+      <c r="C281">
+        <v>249.012</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A282" s="10">
+        <v>40299</v>
+      </c>
+      <c r="B282">
+        <v>147.03799999999899</v>
+      </c>
+      <c r="C282">
+        <v>248.92500000000001</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A283" s="10">
+        <v>40330</v>
+      </c>
+      <c r="B283">
+        <v>147.70400000000001</v>
+      </c>
+      <c r="C283">
+        <v>248.999</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A284" s="10">
+        <v>40360</v>
+      </c>
+      <c r="B284">
+        <v>147.56399999999999</v>
+      </c>
+      <c r="C284">
+        <v>249.126</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A285" s="10">
+        <v>40391</v>
+      </c>
+      <c r="B285">
+        <v>146.428</v>
+      </c>
+      <c r="C285">
+        <v>249.024</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A286" s="10">
+        <v>40422</v>
+      </c>
+      <c r="B286">
+        <v>144.60900000000001</v>
+      </c>
+      <c r="C286">
+        <v>249.36799999999999</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A287" s="10">
+        <v>40452</v>
+      </c>
+      <c r="B287">
+        <v>143.13</v>
+      </c>
+      <c r="C287">
+        <v>249.61799999999999</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A288" s="10">
+        <v>40483</v>
+      </c>
+      <c r="B288">
+        <v>141.821</v>
+      </c>
+      <c r="C288">
+        <v>250.31700000000001</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A289" s="10">
+        <v>40513</v>
+      </c>
+      <c r="B289">
+        <v>140.63200000000001</v>
+      </c>
+      <c r="C289">
+        <v>250.98599999999999</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A290" s="10">
+        <v>40544</v>
+      </c>
+      <c r="B290">
+        <v>139.041</v>
+      </c>
+      <c r="C290">
+        <v>251.55500000000001</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A291" s="10">
+        <v>40575</v>
+      </c>
+      <c r="B291">
+        <v>137.73699999999999</v>
+      </c>
+      <c r="C291">
+        <v>251.82900000000001</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A292" s="10">
+        <v>40603</v>
+      </c>
+      <c r="B292">
+        <v>137.78899999999999</v>
+      </c>
+      <c r="C292">
+        <v>252.14500000000001</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A293" s="10">
+        <v>40634</v>
+      </c>
+      <c r="B293">
+        <v>139.15899999999999</v>
+      </c>
+      <c r="C293">
+        <v>252.221</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A294" s="10">
+        <v>40664</v>
+      </c>
+      <c r="B294">
+        <v>140.69200000000001</v>
+      </c>
+      <c r="C294">
+        <v>252.393</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A295" s="10">
+        <v>40695</v>
+      </c>
+      <c r="B295">
+        <v>141.94399999999999</v>
+      </c>
+      <c r="C295">
+        <v>252.59200000000001</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A296" s="10">
+        <v>40725</v>
+      </c>
+      <c r="B296">
+        <v>142.34299999999999</v>
+      </c>
+      <c r="C296">
+        <v>253.08500000000001</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A297" s="10">
+        <v>40756</v>
+      </c>
+      <c r="B297">
+        <v>141.78700000000001</v>
+      </c>
+      <c r="C297">
+        <v>254.00299999999999</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A298" s="10">
+        <v>40787</v>
+      </c>
+      <c r="B298">
+        <v>140.16999999999999</v>
+      </c>
+      <c r="C298">
+        <v>254.62799999999999</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A299" s="10">
+        <v>40817</v>
+      </c>
+      <c r="B299">
+        <v>138.411</v>
+      </c>
+      <c r="C299">
+        <v>255.65100000000001</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A300" s="10">
+        <v>40848</v>
+      </c>
+      <c r="B300">
+        <v>136.667</v>
+      </c>
+      <c r="C300">
+        <v>256.36700000000002</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A301" s="10">
+        <v>40878</v>
+      </c>
+      <c r="B301">
+        <v>135.16800000000001</v>
+      </c>
+      <c r="C301">
+        <v>257.18900000000002</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A302" s="10">
+        <v>40909</v>
+      </c>
+      <c r="B302">
+        <v>134.16800000000001</v>
+      </c>
+      <c r="C302">
+        <v>257.714</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A303" s="10">
+        <v>40940</v>
+      </c>
+      <c r="B303">
+        <v>133.99600000000001</v>
+      </c>
+      <c r="C303">
+        <v>258.18400000000003</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A304" s="10">
+        <v>40969</v>
+      </c>
+      <c r="B304">
+        <v>135.864</v>
+      </c>
+      <c r="C304">
+        <v>258.56900000000002</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A305" s="10">
+        <v>41000</v>
+      </c>
+      <c r="B305">
+        <v>138.47200000000001</v>
+      </c>
+      <c r="C305">
+        <v>258.92200000000003</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A306" s="10">
+        <v>41030</v>
+      </c>
+      <c r="B306">
+        <v>141.05000000000001</v>
+      </c>
+      <c r="C306">
+        <v>259.23099999999999</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A307" s="10">
+        <v>41061</v>
+      </c>
+      <c r="B307">
+        <v>143.17099999999999</v>
+      </c>
+      <c r="C307">
+        <v>259.40699999999998</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A308" s="10">
+        <v>41091</v>
+      </c>
+      <c r="B308">
+        <v>144.28399999999999</v>
+      </c>
+      <c r="C308">
+        <v>260.10700000000003</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A309" s="10">
+        <v>41122</v>
+      </c>
+      <c r="B309">
+        <v>144.70699999999999</v>
+      </c>
+      <c r="C309">
+        <v>260.67700000000002</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A310" s="10">
+        <v>41153</v>
+      </c>
+      <c r="B310">
+        <v>144.36000000000001</v>
+      </c>
+      <c r="C310">
+        <v>261.42099999999999</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A311" s="10">
+        <v>41183</v>
+      </c>
+      <c r="B311">
+        <v>143.97</v>
+      </c>
+      <c r="C311">
+        <v>262.70699999999999</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A312" s="10">
+        <v>41214</v>
+      </c>
+      <c r="B312">
+        <v>143.96199999999999</v>
+      </c>
+      <c r="C312">
+        <v>263.36500000000001</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A313" s="10">
+        <v>41244</v>
+      </c>
+      <c r="B313">
+        <v>143.87</v>
+      </c>
+      <c r="C313">
+        <v>264.09800000000001</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A314" s="10">
+        <v>41275</v>
+      </c>
+      <c r="B314">
+        <v>144.31299999999999</v>
+      </c>
+      <c r="C314">
+        <v>264.7</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A315" s="10">
+        <v>41306</v>
+      </c>
+      <c r="B315">
+        <v>145.16200000000001</v>
+      </c>
+      <c r="C315">
+        <v>265.25599999999997</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A316" s="10">
+        <v>41334</v>
+      </c>
+      <c r="B316">
+        <v>147.96100000000001</v>
+      </c>
+      <c r="C316">
+        <v>265.82100000000003</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A317" s="10">
+        <v>41365</v>
+      </c>
+      <c r="B317">
+        <v>150.97</v>
+      </c>
+      <c r="C317">
+        <v>265.98399999999998</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A318" s="10">
+        <v>41395</v>
+      </c>
+      <c r="B318">
+        <v>153.86099999999999</v>
+      </c>
+      <c r="C318">
+        <v>266.55900000000003</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A319" s="10">
+        <v>41426</v>
+      </c>
+      <c r="B319">
+        <v>156.43</v>
+      </c>
+      <c r="C319">
+        <v>266.90499999999997</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A320" s="10">
+        <v>41456</v>
+      </c>
+      <c r="B320">
+        <v>158.29</v>
+      </c>
+      <c r="C320">
+        <v>267.48200000000003</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A321" s="10">
+        <v>41487</v>
+      </c>
+      <c r="B321">
+        <v>159.398</v>
+      </c>
+      <c r="C321">
+        <v>268.505</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A322" s="10">
+        <v>41518</v>
+      </c>
+      <c r="B322">
+        <v>159.67599999999999</v>
+      </c>
+      <c r="C322">
+        <v>269.137</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A323" s="10">
+        <v>41548</v>
+      </c>
+      <c r="B323">
+        <v>159.55799999999999</v>
+      </c>
+      <c r="C323">
+        <v>269.95999999999998</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A324" s="10">
+        <v>41579</v>
+      </c>
+      <c r="B324">
+        <v>159.364</v>
+      </c>
+      <c r="C324">
+        <v>270.69799999999998</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A325" s="10">
+        <v>41609</v>
+      </c>
+      <c r="B325">
+        <v>159.28100000000001</v>
+      </c>
+      <c r="C325">
+        <v>271.68799999999999</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A326" s="10">
+        <v>41640</v>
+      </c>
+      <c r="B326">
+        <v>159.37</v>
+      </c>
+      <c r="C326">
+        <v>272.31700000000001</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A327" s="10">
+        <v>41671</v>
+      </c>
+      <c r="B327">
+        <v>159.87299999999999</v>
+      </c>
+      <c r="C327">
+        <v>272.733</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A328" s="10">
+        <v>41699</v>
+      </c>
+      <c r="B328">
+        <v>161.19</v>
+      </c>
+      <c r="C328">
+        <v>273.48599999999999</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A329" s="10">
+        <v>41730</v>
+      </c>
+      <c r="B329">
+        <v>162.97</v>
+      </c>
+      <c r="C329">
+        <v>274.10000000000002</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A330" s="10">
+        <v>41760</v>
+      </c>
+      <c r="B330">
+        <v>164.685</v>
+      </c>
+      <c r="C330">
+        <v>274.70999999999998</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A331" s="10">
+        <v>41791</v>
+      </c>
+      <c r="B331">
+        <v>166.214</v>
+      </c>
+      <c r="C331">
+        <v>275.32100000000003</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A332" s="10">
+        <v>41821</v>
+      </c>
+      <c r="B332">
+        <v>167.13900000000001</v>
+      </c>
+      <c r="C332">
+        <v>276.24799999999999</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A333" s="10">
+        <v>41852</v>
+      </c>
+      <c r="B333">
+        <v>167.45400000000001</v>
+      </c>
+      <c r="C333">
+        <v>277.048</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A334" s="10">
+        <v>41883</v>
+      </c>
+      <c r="B334">
+        <v>167.245</v>
+      </c>
+      <c r="C334">
+        <v>277.99799999999999</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A335" s="10">
+        <v>41913</v>
+      </c>
+      <c r="B335">
+        <v>166.91399999999999</v>
+      </c>
+      <c r="C335">
+        <v>278.98500000000001</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A336" s="10">
+        <v>41944</v>
+      </c>
+      <c r="B336">
+        <v>166.66200000000001</v>
+      </c>
+      <c r="C336">
+        <v>280.12299999999999</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A337" s="10">
+        <v>41974</v>
+      </c>
+      <c r="B337">
+        <v>166.465</v>
+      </c>
+      <c r="C337">
+        <v>280.87400000000002</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A338" s="10">
+        <v>42005</v>
+      </c>
+      <c r="B338">
+        <v>166.255</v>
+      </c>
+      <c r="C338">
+        <v>281.572</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A339" s="10">
+        <v>42036</v>
+      </c>
+      <c r="B339">
+        <v>166.637</v>
+      </c>
+      <c r="C339">
+        <v>282.38900000000001</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A340" s="10">
+        <v>42064</v>
+      </c>
+      <c r="B340">
+        <v>168.09399999999999</v>
+      </c>
+      <c r="C340">
+        <v>283.13</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A341" s="10">
+        <v>42095</v>
+      </c>
+      <c r="B341">
+        <v>169.97299999999899</v>
+      </c>
+      <c r="C341">
+        <v>283.59800000000001</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A342" s="10">
+        <v>42125</v>
+      </c>
+      <c r="B342">
+        <v>171.85299999999901</v>
+      </c>
+      <c r="C342">
+        <v>284.245</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A343" s="10">
+        <v>42156</v>
+      </c>
+      <c r="B343">
+        <v>173.452</v>
+      </c>
+      <c r="C343">
+        <v>285.03100000000001</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A344" s="10">
+        <v>42186</v>
+      </c>
+      <c r="B344">
+        <v>174.49700000000001</v>
+      </c>
+      <c r="C344">
+        <v>286.08999999999997</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A345" s="10">
+        <v>42217</v>
+      </c>
+      <c r="B345">
+        <v>174.94</v>
+      </c>
+      <c r="C345">
+        <v>287.06799999999998</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A346" s="10">
+        <v>42248</v>
+      </c>
+      <c r="B346">
+        <v>175.048</v>
+      </c>
+      <c r="C346">
+        <v>288.30599999999998</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A347" s="10">
+        <v>42278</v>
+      </c>
+      <c r="B347">
+        <v>175.05500000000001</v>
+      </c>
+      <c r="C347">
+        <v>289.428</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A348" s="10">
+        <v>42309</v>
+      </c>
+      <c r="B348">
+        <v>175.149</v>
+      </c>
+      <c r="C348">
+        <v>290.322</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A349" s="10">
+        <v>42339</v>
+      </c>
+      <c r="B349">
+        <v>175.12299999999999</v>
+      </c>
+      <c r="C349">
+        <v>291.20400000000001</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A350" s="10">
+        <v>42370</v>
+      </c>
+      <c r="B350">
+        <v>175.04300000000001</v>
+      </c>
+      <c r="C350">
+        <v>292.00400000000002</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A351" s="10">
+        <v>42401</v>
+      </c>
+      <c r="B351">
+        <v>175.28700000000001</v>
+      </c>
+      <c r="C351">
+        <v>292.77699999999999</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A352" s="10">
+        <v>42430</v>
+      </c>
+      <c r="B352">
+        <v>176.60599999999999</v>
+      </c>
+      <c r="C352">
+        <v>293.48899999999998</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A353" s="10">
+        <v>42461</v>
+      </c>
+      <c r="B353">
+        <v>178.49799999999999</v>
+      </c>
+      <c r="C353">
+        <v>294.17500000000001</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A354" s="10">
+        <v>42491</v>
+      </c>
+      <c r="B354">
+        <v>180.345</v>
+      </c>
+      <c r="C354">
+        <v>295.036</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A355" s="10">
+        <v>42522</v>
+      </c>
+      <c r="B355">
+        <v>181.91800000000001</v>
+      </c>
+      <c r="C355">
+        <v>295.90199999999999</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A356" s="10">
+        <v>42552</v>
+      </c>
+      <c r="B356">
+        <v>183.023</v>
+      </c>
+      <c r="C356">
+        <v>296.86200000000002</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A357" s="10">
+        <v>42583</v>
+      </c>
+      <c r="B357">
+        <v>183.66099999999901</v>
+      </c>
+      <c r="C357">
+        <v>297.916</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A358" s="10">
+        <v>42614</v>
+      </c>
+      <c r="B358">
+        <v>183.95099999999999</v>
+      </c>
+      <c r="C358">
+        <v>298.96199999999999</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A359" s="10">
+        <v>42644</v>
+      </c>
+      <c r="B359">
+        <v>184.02599999999899</v>
+      </c>
+      <c r="C359">
+        <v>300.39999999999998</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A360" s="10">
+        <v>42675</v>
+      </c>
+      <c r="B360">
+        <v>184.239</v>
+      </c>
+      <c r="C360">
+        <v>301.58699999999999</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A361" s="10">
+        <v>42705</v>
+      </c>
+      <c r="B361">
+        <v>184.41</v>
+      </c>
+      <c r="C361">
+        <v>302.73500000000001</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A362" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B362">
+        <v>184.66099999999901</v>
+      </c>
+      <c r="C362">
+        <v>303.46699999999998</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A363" s="10">
+        <v>42767</v>
+      </c>
+      <c r="B363">
+        <v>185.02699999999999</v>
+      </c>
+      <c r="C363">
+        <v>304.21100000000001</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A364" s="10">
+        <v>42795</v>
+      </c>
+      <c r="B364">
+        <v>186.53599999999901</v>
+      </c>
+      <c r="C364">
+        <v>304.86799999999999</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A365" s="10">
+        <v>42826</v>
+      </c>
+      <c r="B365">
+        <v>188.55099999999999</v>
+      </c>
+      <c r="C365">
+        <v>305.47699999999998</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A366" s="10">
+        <v>42856</v>
+      </c>
+      <c r="B366">
+        <v>190.54900000000001</v>
+      </c>
+      <c r="C366">
+        <v>306.37900000000002</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A367" s="10">
+        <v>42887</v>
+      </c>
+      <c r="B367">
+        <v>192.27799999999999</v>
+      </c>
+      <c r="C367">
+        <v>307.31400000000002</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A368" s="10">
+        <v>42917</v>
+      </c>
+      <c r="B368">
+        <v>193.524</v>
+      </c>
+      <c r="C368">
+        <v>308.173</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A369" s="10">
+        <v>42948</v>
+      </c>
+      <c r="B369">
+        <v>194.35900000000001</v>
+      </c>
+      <c r="C369">
+        <v>309.47899999999998</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A370" s="10">
+        <v>42979</v>
+      </c>
+      <c r="B370">
+        <v>194.82900000000001</v>
+      </c>
+      <c r="C370">
+        <v>310.26799999999997</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A371" s="10">
+        <v>43009</v>
+      </c>
+      <c r="B371">
+        <v>195.09299999999999</v>
+      </c>
+      <c r="C371">
+        <v>311.50099999999998</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A372" s="10">
+        <v>43040</v>
+      </c>
+      <c r="B372">
+        <v>195.45699999999999</v>
+      </c>
+      <c r="C372">
+        <v>312.67</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A373" s="10">
+        <v>43070</v>
+      </c>
+      <c r="B373">
+        <v>195.852</v>
+      </c>
+      <c r="C373">
+        <v>313.904</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A374" s="10">
+        <v>43101</v>
+      </c>
+      <c r="B374">
+        <v>196.12</v>
+      </c>
+      <c r="C374">
+        <v>314.78800000000001</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A375" s="10">
+        <v>43132</v>
+      </c>
+      <c r="B375">
+        <v>196.91</v>
+      </c>
+      <c r="C375">
+        <v>315.27699999999999</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A376" s="10">
+        <v>43160</v>
+      </c>
+      <c r="B376">
+        <v>198.57900000000001</v>
+      </c>
+      <c r="C376">
+        <v>315.88299999999998</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A377" s="10">
+        <v>43191</v>
+      </c>
+      <c r="B377">
+        <v>200.62299999999999</v>
+      </c>
+      <c r="C377">
+        <v>316.76299999999998</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A378" s="10">
+        <v>43221</v>
+      </c>
+      <c r="B378">
+        <v>202.46199999999999</v>
+      </c>
+      <c r="C378">
+        <v>317.49</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A379" s="10">
+        <v>43252</v>
+      </c>
+      <c r="B379">
+        <v>204.054</v>
+      </c>
+      <c r="C379">
+        <v>318.31799999999998</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A380" s="10">
+        <v>43282</v>
+      </c>
+      <c r="B380">
+        <v>204.96299999999999</v>
+      </c>
+      <c r="C380">
+        <v>319.351</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A381" s="10">
+        <v>43313</v>
+      </c>
+      <c r="B381">
+        <v>205.34099999999901</v>
+      </c>
+      <c r="C381">
+        <v>320.65100000000001</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A382" s="10">
+        <v>43344</v>
+      </c>
+      <c r="B382">
+        <v>205.38800000000001</v>
+      </c>
+      <c r="C382">
+        <v>321.53300000000002</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A383" s="10">
+        <v>43374</v>
+      </c>
+      <c r="B383">
+        <v>205.38399999999999</v>
+      </c>
+      <c r="C383">
+        <v>322.62799999999999</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A384" s="10">
+        <v>43405</v>
+      </c>
+      <c r="B384">
+        <v>205.12200000000001</v>
+      </c>
+      <c r="C384">
+        <v>323.96800000000002</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A385" s="10">
+        <v>43435</v>
+      </c>
+      <c r="B385">
+        <v>204.71299999999999</v>
+      </c>
+      <c r="C385">
+        <v>324.815</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A386" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B386">
+        <v>204.21700000000001</v>
+      </c>
+      <c r="C386">
+        <v>325.59699999999998</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A387" s="10">
+        <v>43497</v>
+      </c>
+      <c r="B387">
+        <v>204.44499999999999</v>
+      </c>
+      <c r="C387">
+        <v>326.351</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A388" s="10">
+        <v>43525</v>
+      </c>
+      <c r="B388">
+        <v>205.792</v>
+      </c>
+      <c r="C388">
+        <v>327.51299999999998</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A389" s="10">
+        <v>43556</v>
+      </c>
+      <c r="B389">
+        <v>207.70400000000001</v>
+      </c>
+      <c r="C389">
+        <v>328.678</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A390" s="10">
+        <v>43586</v>
+      </c>
+      <c r="B390">
+        <v>209.369</v>
+      </c>
+      <c r="C390">
+        <v>329.33300000000003</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A391" s="10">
+        <v>43617</v>
+      </c>
+      <c r="B391">
+        <v>210.608</v>
+      </c>
+      <c r="C391">
+        <v>330.64800000000002</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A392" s="10">
+        <v>43647</v>
+      </c>
+      <c r="B392">
+        <v>211.36199999999999</v>
+      </c>
+      <c r="C392">
+        <v>331.60500000000002</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A393" s="10">
+        <v>43678</v>
+      </c>
+      <c r="B393">
+        <v>211.72099999999901</v>
+      </c>
+      <c r="C393">
+        <v>332.63799999999998</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A394" s="10">
+        <v>43709</v>
+      </c>
+      <c r="B394">
+        <v>211.899</v>
+      </c>
+      <c r="C394">
+        <v>333.834</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A395" s="10">
+        <v>43739</v>
+      </c>
+      <c r="B395">
+        <v>211.99099999999899</v>
+      </c>
+      <c r="C395">
+        <v>334.68</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A396" s="10">
+        <v>43770</v>
+      </c>
+      <c r="B396">
+        <v>212.12799999999999</v>
+      </c>
+      <c r="C396">
+        <v>335.81900000000002</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A397" s="10">
+        <v>43800</v>
+      </c>
+      <c r="B397">
+        <v>212.25799999999899</v>
+      </c>
+      <c r="C397">
+        <v>336.78899999999999</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A398" s="10">
+        <v>43831</v>
+      </c>
+      <c r="B398">
+        <v>212.41800000000001</v>
+      </c>
+      <c r="C398">
+        <v>337.82499999999999</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A399" s="10">
+        <v>43862</v>
+      </c>
+      <c r="B399">
+        <v>213.238</v>
+      </c>
+      <c r="C399">
+        <v>338.61599999999999</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A400" s="10">
+        <v>43891</v>
+      </c>
+      <c r="B400">
+        <v>215.21700000000001</v>
+      </c>
+      <c r="C400">
+        <v>339.51900000000001</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A401" s="10">
+        <v>43922</v>
+      </c>
+      <c r="B401">
+        <v>217.26499999999999</v>
+      </c>
+      <c r="C401">
+        <v>340.13499999999999</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A402" s="10">
+        <v>43952</v>
+      </c>
+      <c r="B402">
+        <v>218.51599999999999</v>
+      </c>
+      <c r="C402">
+        <v>340.81099999999998</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A403" s="10">
+        <v>43983</v>
+      </c>
+      <c r="B403">
+        <v>219.84099999999901</v>
+      </c>
+      <c r="C403">
+        <v>341.29399999999998</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A404" s="10">
+        <v>44013</v>
+      </c>
+      <c r="B404">
+        <v>221.59399999999999</v>
+      </c>
+      <c r="C404">
+        <v>341.95</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A405" s="10">
+        <v>44044</v>
+      </c>
+      <c r="B405">
+        <v>224.07400000000001</v>
+      </c>
+      <c r="C405">
+        <v>342.44400000000002</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A406" s="10">
+        <v>44075</v>
+      </c>
+      <c r="B406">
+        <v>226.83199999999999</v>
+      </c>
+      <c r="C406">
+        <v>342.91</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A407" s="10">
+        <v>44105</v>
+      </c>
+      <c r="B407">
+        <v>229.851</v>
+      </c>
+      <c r="C407">
+        <v>343.61500000000001</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A408" s="10">
+        <v>44136</v>
+      </c>
+      <c r="B408">
+        <v>232.364</v>
+      </c>
+      <c r="C408">
+        <v>344.03899999999999</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A409" s="10">
+        <v>44166</v>
+      </c>
+      <c r="B409">
+        <v>234.416</v>
+      </c>
+      <c r="C409">
+        <v>344.45499999999998</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A410" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B410">
+        <v>236.488</v>
+      </c>
+      <c r="C410">
+        <v>344.75799999999998</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A411" s="10">
+        <v>44228</v>
+      </c>
+      <c r="B411">
+        <v>239.25599999999901</v>
+      </c>
+      <c r="C411">
+        <v>345.24200000000002</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A412" s="10">
+        <v>44256</v>
+      </c>
+      <c r="B412">
+        <v>244.25799999999899</v>
+      </c>
+      <c r="C412">
+        <v>345.71699999999998</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A413" s="10">
+        <v>44287</v>
+      </c>
+      <c r="B413">
+        <v>249.86699999999999</v>
+      </c>
+      <c r="C413">
+        <v>346.267</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A414" s="10">
+        <v>44317</v>
+      </c>
+      <c r="B414">
+        <v>255.49599999999899</v>
+      </c>
+      <c r="C414">
+        <v>347.01600000000002</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A415" s="10">
+        <v>44348</v>
+      </c>
+      <c r="B415">
+        <v>261.221</v>
+      </c>
+      <c r="C415">
+        <v>347.83300000000003</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A416" s="10">
+        <v>44378</v>
+      </c>
+      <c r="B416">
+        <v>265.54899999999998</v>
+      </c>
+      <c r="C416">
+        <v>348.46899999999999</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A417" s="10">
+        <v>44409</v>
+      </c>
+      <c r="B417">
+        <v>268.822</v>
+      </c>
+      <c r="C417">
+        <v>349.71</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A418" s="10">
+        <v>44440</v>
+      </c>
+      <c r="B418">
+        <v>271.47399999999999</v>
+      </c>
+      <c r="C418">
+        <v>351.255</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A419" s="10">
+        <v>44470</v>
+      </c>
+      <c r="B419">
+        <v>273.68799999999999</v>
+      </c>
+      <c r="C419">
+        <v>352.892</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A420" s="10">
+        <v>44501</v>
+      </c>
+      <c r="B420">
+        <v>276.06200000000001</v>
+      </c>
+      <c r="C420">
+        <v>354.52600000000001</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A421" s="10">
+        <v>44531</v>
+      </c>
+      <c r="B421">
+        <v>278.64</v>
+      </c>
+      <c r="C421">
+        <v>355.93099999999998</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A422" s="10">
+        <v>44562</v>
+      </c>
+      <c r="B422">
+        <v>282.015999999999</v>
+      </c>
+      <c r="C422">
+        <v>357.73700000000002</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A423" s="10">
+        <v>44593</v>
+      </c>
+      <c r="B423">
+        <v>287.26299999999998</v>
+      </c>
+      <c r="C423">
+        <v>359.62700000000001</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A424" s="10">
+        <v>44621</v>
+      </c>
+      <c r="B424">
+        <v>295.10899999999998</v>
+      </c>
+      <c r="C424">
+        <v>361.08300000000003</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A425" s="10">
+        <v>44652</v>
+      </c>
+      <c r="B425">
+        <v>301.79700000000003</v>
+      </c>
+      <c r="C425">
+        <v>362.95100000000002</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A426" s="10">
+        <v>44682</v>
+      </c>
+      <c r="B426">
+        <v>306.57799999999997</v>
+      </c>
+      <c r="C426">
+        <v>365.11599999999999</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A427" s="10">
+        <v>44713</v>
+      </c>
+      <c r="B427">
+        <v>308.35599999999999</v>
+      </c>
+      <c r="C427">
+        <v>367.92700000000002</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A428" s="10">
+        <v>44743</v>
+      </c>
+      <c r="B428">
+        <v>307.15499999999997</v>
+      </c>
+      <c r="C428">
+        <v>370.44799999999998</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A429" s="10">
+        <v>44774</v>
+      </c>
+      <c r="B429">
+        <v>303.66199999999998</v>
+      </c>
+      <c r="C429">
+        <v>373.28300000000002</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A430" s="10">
+        <v>44805</v>
+      </c>
+      <c r="B430">
+        <v>300.53199999999998</v>
+      </c>
+      <c r="C430">
+        <v>376.56900000000002</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A431" s="10">
+        <v>44835</v>
+      </c>
+      <c r="B431">
+        <v>298.86599999999999</v>
+      </c>
+      <c r="C431">
+        <v>379.43599999999998</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A432" s="10">
+        <v>44866</v>
+      </c>
+      <c r="B432">
+        <v>297.09199999999998</v>
+      </c>
+      <c r="C432">
+        <v>382.56200000000001</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A433" s="10">
+        <v>44896</v>
+      </c>
+      <c r="B433">
+        <v>294.67899999999997</v>
+      </c>
+      <c r="C433">
+        <v>385.649</v>
       </c>
     </row>
   </sheetData>
@@ -24967,12 +29750,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024A92190D758C14CABA06EB5DDDCFAB6" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d4d4151efdceb84e9b5f2f7e6aee3da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdcab5d-de70-4d4a-a9b3-2de08f1afc7f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23ee0c930fb979ef27d10e53ad7fa985" ns2:_="">
     <xsd:import namespace="9bdcab5d-de70-4d4a-a9b3-2de08f1afc7f"/>
@@ -25150,6 +29927,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA1FB5EB-EFE3-481E-8ABF-D5CC8531030B}">
   <ds:schemaRefs>
@@ -25159,15 +29942,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{322045DD-D7EC-42A1-AB1C-7B83E56C54D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1B4A3D3-7D1D-4E66-8021-5662A79A0B97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25183,4 +29957,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{322045DD-D7EC-42A1-AB1C-7B83E56C54D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>